<commit_message>
limit volunteers, lidar com turnos extra
</commit_message>
<xml_diff>
--- a/pessoas-big.xlsx
+++ b/pessoas-big.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/b68001cfe7d3a722/Ambiente de Trabalho/jeec/schedule_otimization/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="53" documentId="13_ncr:1_{5D30E52C-EC23-404F-9A3E-2E7A92E17B81}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{737840E1-FE0A-4626-84BA-FCBD3E9769C8}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="13_ncr:1_{DBA8300C-A3D3-4714-A3DA-56C05CC7D6ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{38B85031-6538-48E3-8221-F9A6FFB0EDA4}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{ED6C3682-79FE-4B69-93D1-DE209828B5EC}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$74</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Folha1!$A$1:$C$72</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="151">
   <si>
     <t>Nome</t>
   </si>
@@ -281,325 +281,217 @@
     <t>Vol30</t>
   </si>
   <si>
-    <t>Vol31</t>
-  </si>
-  <si>
-    <t>Vol32</t>
-  </si>
-  <si>
-    <t>Vol33</t>
-  </si>
-  <si>
-    <t>Vol34</t>
-  </si>
-  <si>
-    <t>Vol35</t>
-  </si>
-  <si>
-    <t>Vol36</t>
-  </si>
-  <si>
-    <t>Vol37</t>
-  </si>
-  <si>
-    <t>Vol38</t>
-  </si>
-  <si>
-    <t>Vol39</t>
-  </si>
-  <si>
-    <t>Vol40</t>
-  </si>
-  <si>
-    <t>Vol41</t>
-  </si>
-  <si>
-    <t>Vol42</t>
-  </si>
-  <si>
-    <t>Vol43</t>
-  </si>
-  <si>
-    <t>Vol44</t>
-  </si>
-  <si>
-    <t>Vol45</t>
-  </si>
-  <si>
-    <t>Vol46</t>
-  </si>
-  <si>
-    <t>Vol47</t>
-  </si>
-  <si>
-    <t>Vol48</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,1,0,1,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,0,0,1,0,1,1,1,1,1,1,1,1,0,1,1,1,1,0,0,0,1,1,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,0,1,1,1,1,0,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,1,1,0,1,0,1,1,0,0,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,0,1,1,1,1,1,0,0,1,0,1,0,0,1,0,1,0,1,1,1,0,0,0,1,0,0,0,0,0,1,1,1,1,0,0,0,1,1,1,1,0,0,1,0,1,0,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,1,1,1,0,0,0,0,0,0,1,0,1,0,0,1,0,1,1,1,1,0,0,0,0,0,0,1,0,1,0,1,1,0,1,1,0,0,0,1,1,0,0,0,1,0,0,1,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,0,0,0,0,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,1,1,1,0,0,0,0,0,1,0,1,1,1,1,1,1,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,0,1,0,1,0,1,0,1,1,1,1,1,0,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,1,1,1,1,0,0,1,1,1,0,0,1,0,1,0,1,1,1,1,1,0,0,0,1,0,0,1,0,0,0,1,1,0,1,1,0,1,1,0,0,0,0,1,1,0,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,0,1,1,1,1,0,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,1,0,1,1,0,0,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,0,0,0,1,0,1,0,1,1,1,1,1,0,1,0,1,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0,1,1,0,1,1,1,0,1,0,1,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,1,0,0,1,1,1,0,0,1,0,0,0,0,0,0,1,0,0,0,1,1,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,1,1,1,0,0,1,1,0,0,1,1,1,0,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,0,1,0,0,1,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,1,0,0,1,1,0,0,0,0,1,0,0,1,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,1,0,0,0,0,1,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,1,0,0,0,0,0,1,0,1,1,1,1,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,1,0,1,1,0,1,0,0,1,0,0,1,1,1,1,0,1,1,0,0,1,1,0,1,1,0,0,1,1,1,1,0,1,1,0,1,0,0,1,0,0,0,0,0,1,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,1,0,1,1,1,1,1,0,1,1,1,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,0,1,0,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,0,0,0,1,0,1,1,0,1,1,0,0,1,1,0,0,0,1,0,0,1,0,0,1,1,1,0,1,1,0,0,1,1,1,1,0,0,0,1,1,1,1,1,0,1,1,0,1,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,0,0,1,1,1,1,1,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,1,0,1,0,0,1,1,0,0,1,0,1,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,1,0,1,1,1,1,0,1,1,1,1,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,0,1,0,0,1,1,1,0,0,1,1,0,1,0,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,1,0,1,1,0,0,1,0,0,0,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,1,1,1,1,0,1,0,1,1,1,1,0,1,0,0,0,1,1,1,1,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0,1,0,1,0,0,0,0,0,1,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,0,0,1,1,0,0,0,0,0,1,0,0,1,1,0,0,0,1,1,1,0,0,0,1,0,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,1,0,1,1,1,0,1,1,1,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,0,0,0,0,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,1,0,0,1,0,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,1,0,0,1,0,0,0,1,0,1,0,0,1,0,0,1,0,0,0,0,0,1,1,1,0,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,1,1,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0,1,1,1,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,1,0,0,0,1,0,0,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,1,0,1,0,0,0,1,1,1,0,1,0,1,0,0,0,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,1,0,0,1,1,1,1,0,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,0,0,1,0,0,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,1,0,0,0,0,1,1,0,0,0,0,0,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,0,0,1,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,0,0,1,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,0,1,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,1,0,0,0,1,1,0,1,1,1,1,1,0,0,1,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,1,1,1,1,1,1,0,0,0,1,0,1,0,0,0,1,0,0,0,1,0,1,1,1,0]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,1,0,0,1,0,1,0,1,0,1,0,1,1,1,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,0,1,0,1,0,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,0,1,1,0,1,0,0,1,0,1,0,0,1,0,0,0,1,1,1,0,0,0,1,0,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,1,1,0,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,1,1,1,0,1,1,0,0,1,0,0,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,0,1,1,0,0,1,0,0,1,1,1,1,0,1,1,0,1,1,1,0,0,1,0,1,1,1,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,0,0,0,1,1,0,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,0,0,0,0,0,1,1,0,1,1,0,0,1,1,0,1,1,1,0,0,0,1,0,1,1,1,1,0,1,0,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,1,1,0,0,0,0,0,0,1,0,1,1,1,0,1,0,0,0,1,1,1,0,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,1,1,0,0,1,1,0]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,1,0,1,0,0,1,0,1,0,1,0,1,0,0,0,0,0,1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,1,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,1,1,1,0,1,0,0,0,1,1,0,0,1,1,1,1,0,1,1,1,1,0,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,0,1,0,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,1,1,0,0,1,0,1,0,1,1,1,0,1,1,0,0,0,0,1,0,0,1,0,1,1,0,0,1,1,0,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,1,0,1,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,0,1,1,0,0,0,1,1,1,1,1,1,1,0,1,0,1,1,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,1,1,0]</t>
-  </si>
-  <si>
-    <t>[0,1,1,1,0,0,1,0,1,0,1,0,1,1,0,0,0,0,1,0,1,0,1,1,1,0,1,0,0,0,0,0,1,1,0,0,1,0,1,0,0,1,0,0,0,0,0,0,1,0,1,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,1,0,0,1,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,0,0,1,0,0,0,0,1,0,1,1,0,0,0,0,0,0,1,1,0,1,0,0,1,1,1,0,0,0,1,1,0,1,0,0,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,0,1,1,0,1,0,0,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,1,1,0,1,0,1,0,0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,0,0,0,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,1,0,1,0,1,0,0,1,1,1,0,0,0,0,0,0,1,1,0,0,0,1,1,0,0,0,0,0,1,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,0,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,0,0,1,1,0,0,1,0,0,1,0,1,1,0,1,0,0,1,1,1,1,0,0,0,1,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,1,0,0,0,0,0,1,1,0,1,1,1,0,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,0,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,0,1,1,0,0,0,1,0,0,0,0,0,0,0,1,1,0,1,1,1,1,0,0,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,1,1,0,0,0,0,0,0,1,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,1,0,0,1,0,0,1,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,0,1,1,0,0,0,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,0,0,0,1,1,0,0,1,1,1,0,0,0,0,1,0,1,0,0,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,0,1,0,1,1,1,1,1,1,0,0,1,0,0,1,0,0,0,0,1,1,0,1,0,1,0,1,1,0,1,1,0,1,0,0,1,0,1,1,0,1,0,0,1,0,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,1,1,0,1,0,0,1,1,1,1,1,0,0,1,1,1,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,0,1,0,1,0,1,0,1,0,0,0,0,1,1,1,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,0,0,1,1,0,0,0,0,0,1,1,0,1,0,1,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,0,0,1,1,1,0,0,0,0,1,1,1,0,0,1,0,1,1,0,1,0,1,0,1,0,0,0,1,1,0,0,0,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,0,1,1,1,0,1,0,0,1,1,1,1,0,0,0,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,1,0,1,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,1,1,1,0,0,1,1,0,1,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,1,0,1,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,0,0,1,1,0,0,1,1,1,0,1,0,1,0,1,1,0,1,0,0,0,1,1,0,1,1,0,0,1,1,0,0,1,1,0,0,1,0,1,1,0,0,0,0,0,0,0,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,1,0,1,1,0,1,1,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,0,1,0,1,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,1,0,0,1,0,1,1,0,0,1,1,0,1,0,0,0,1,0,1,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,1,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,0,1,0,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,0,1,0,0,0,1,1,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,1,0,0,1,0,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,0,1,0,1,1,0,0,1,0,1,0,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,1,1,1,0,0,1,0,0,0,0,1,1,1,0,0,0,0,1,0,0,0,0,1,0,1,0,0,1,1,1,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,0,0,0,1,0,0,1,1,1,1,0,1,1,1,0,0,1,0,1,1,0,1,1,0,1,1,0,1,0,0,0,1,0,0,0,1,1,1,1,0,0,0,0,0,1,1,1,0,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,1,0,1,0,1,0,1,0,1,0,1,1,1,0,1,1,0,1,1,0,1,0,1,0,1,0,1,0,0,0,1,0,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,1,1,0,1,1,0,1,0,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,1,0,1,1,0,0,0,1,1,1,0,1,0,0,0,1,0,1,1,0,1,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,0,1,0,0,0,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,1,1,1,1,0,0,1,1,0,1,0,0,0,1,1,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,0,1,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,0,1,0,0,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,1,0,0,1,1,0,1,0,0,1,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,1,0,1,0,1,1,0,0,1,0,1,1,0,1,1,0,1,0,1,1,0,0,0,1,1,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,0,0,1,0,0,1,0,1,0,1,0,1,1,1,0,0,1,0,0,1,1,0,1,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,0,1,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,1,1,1,0,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,0,0,1,1,0,1,0,0,0,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,0,1,0]</t>
-  </si>
-  <si>
-    <t>[0,1,1,1,0,0,1,0,1,1,1,1,1,1,0,1,0,0,1,0,0,1,1,1,1,0,0,1,1,1,0,1,0,0,1,1,0,0,0,0,0,1,1,1,0,1,1,1,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,1,1,0,1,0,0,0,0,0,0,1,0,0,0,0,0,0,1,1,1,0,1,1,0,1,1,1,1,0,0,1,1,1,0,0,1,1,1,1,0,0,0,1,0,0,0,0,0,1,1,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,1,0,1,1,1,0,0,1,1,0,0,1,1,0,0,0,1,1,0,0,1,1,1,1,0,0,0,0,0,1,1,0,0,1,1,1,1,1,1,0,0,0,1,1,0,0,0,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,1,0,0,0,0,0,1,1,1,1,1,1,1,1,1,0,1,1,0,1,0,1,0,0,1,1,0,1,1,1,0,0,0,1,1,1,1,0,0,0,0,1,0,1,1,1,1,0,1,1,0,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,1,1,0,1,0,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,0,1,0,1,1,0,0,1,0,1,0,0,0,0,0,0,1,0,1,1,1,1,1,0,1,0,0,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,1,1,0,0,1,0,0,1,1,0,1,1,1,1,1,0,1,0,1,0,1,1,1,1,0,0,0,0,0,0,0,1,0,0,0,0,1,0,0,0,0,1,0,1,0,1,1,1,1,1,1,0,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,0,1,0,1,0,0,1,1,1,1,1,0,1,1,1,0,1,0,0,1,1,0,1,0,0,1,1,0,0,1,0,1,0,0,0,0,1,1,0,0,0,0,1,0,0,0,0,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,1,1,0,1,0,1,0,1,0,1,1,0,0,1,0,1,0,0,1,0,0,1,1,0,1,1,1,0,0,0,0,0,0,0,1,0,0,0,1,1,1,1,0,1,1,1,0,1,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,1,1,1,1,0,0,0,0,1,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1,1,1,1,0,1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,1,1,1,1,1,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,0,0,1,0,0,1,0,0,1,0,1,1,0,0,1,1,1,1,1,0,1,0,1,0,1,1,0,0,1,0,1,1,1,1,0,1,0,0,0,0,0,1,0,0,1,1,1,0,1,1,0]</t>
-  </si>
-  <si>
-    <t>[0,1,0,1,0,1,1,1,0,1,1,0,1,1,1,0,1,0,1,1,1,0,1,1,0,1,1,1,1,1,1,0,1,0,0,0,0,0,1,0,0,0,1,0,0,1,0,1,0,1,1,0,0,1]</t>
-  </si>
-  <si>
-    <t>[0,0,0,0,1,0,0,0,1,1,0,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,0,0,0,1,0,0,1,1,1,0,0,0,1,1,1,1,0,0,1,1,0,0,0,1,1,1,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,1,0,1,1,1,0,1,1,1,0,1,0,1,0,0,0,1,1,0,0,0,1,0,0,0,0,0,0,1,0,0,1,1,0,0,0,0,1,1,1,1,1,1,1,0,0,1,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,0,1,0,1,0,1,0,1,0,1,0,0,1,1,1,1,1,0,1,1,1,0,1,1,1,1,1,1,0,1,0,0,1,1,1,1,0,0,1,1,0,1,1,0,0,1,0,0,1,1,1,1]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,0,1,0,0,1,0,1,0,0,1,0,1,0,0,1,1,0,0,1,0,1,0,1,1,1,0,1,0,0,1,1,1,1,0,0,0,0,0,1,1,0,0,1,1,1,1,0,0,1,1]</t>
-  </si>
-  <si>
-    <t>[1,0,1,1,1,0,0,0,1,0,1,0,1,1,0,1,1,1,1,0,0,0,0,0,1,1,1,1,1,1,0,1,0,1,1,0,0,1,1,0,1,1,0,1,1,0,1,0,1,1,0,0,1,0]</t>
-  </si>
-  <si>
-    <t>[0,0,1,1,0,1,0,0,0,1,1,1,0,1,1,0,1,0,1,1,1,0,0,0,1,1,1,0,1,1,0,0,1,1,0,0,0,0,0,1,0,0,1,0,1,1,1,0,1,0,1,1,0,0]</t>
-  </si>
-  <si>
-    <t>[1,1,0,1,1,0,0,0,1,0,1,0,0,1,1,1,1,0,1,1,0,0,0,1,0,0,1,1,1,1,0,1,0,1,0,1,0,0,1,1,1,1,0,0,0,1,0,1,1,0,0,0,1,0]</t>
+    <t>[0,0,0,1,1,0,1,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,0,0,1,0,1,1,1,1,1,1,1,1,0,1,1,1,1,0,0,0,1,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,1,1,1,1,0,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,1,1,0,1,0,1,1,0,0,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,0,1,1,1,1,1,0,0,1,0,1,0,0,1,0,1,0,1,1,1,0,0,0,1,0,0,0,0,0,1,1,1,1,0,0,0,1,1,1,1,0,0,1,0,1,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,1,1,1,0,0,0,0,0,0,1,0,1,0,0,1,0,1,1,1,1,0,0,0,0,0,0,1,0,1,0,1,1,0,1,1,0,0,0,1,1,0,0,0,1,0,0,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,0,0,0,0,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,1,1,0,1,1,1,0,1,0,0,1,1,0,1,1,1,1,0,1,1,1,0,0,0,0,0,1,0,1,1,1,1,1,1,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,0,1,0,1,0,1,0,1,1,1,1,1,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,1,1,1,0,0,1,1,1,0,0,1,0,1,0,1,1,1,1,1,0,0,0,1,0,0,1,0,0,0,1,1,0,1,1,0,1,1,0,0,0,0,1,1,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,0,1,1,0,0,0,1,0,1,1,0,1,1,0,1,1,1,1,0,0,0,0,0,1,1,0,1,0,0,1,0,0,0,0,0,0,1,1,1,1,1,0,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,1,1,1,1,0,1,1,1,1,0,0,0,0,0,0,0,0,0,1,0,1,0,1,1,1,1,1,0,1,0,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,1,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,1,0,1,1,1,0,1,0,1,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,1,0,0,1,1,1,0,0,1,0,0,0,0,0,0,1,0,0,0,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,1,0,0,1,1,0,0,1,1,1,0,1,1,1,0,1,1,1,0,1,0,0,0,1,1,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,0,1,0,0,1,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,1,0,0,1,1,0,0,0,0,1,0,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,0,0,0,0,1,0,0,0,0,1,1,0,0,0,1,0,0,0,0,0,1,1,0,0,0,0,0,1,0,1,1,1,1,0,0,0,1,1,1,1,1,1,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,0,1,0,0,1,0,0,1,1,1,1,0,1,1,0,0,1,1,0,1,1,0,0,1,1,1,1,0,1,1,0,1,0,0,1,0,0,0,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,1,1,0,1,0,1,1,0,0,1,1,1,0,1,0,1,1,1,1,1,0,1,1,1,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,0,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,0,1,0,1,1,0,1,1,0,0,1,1,0,0,0,1,0,0,1,0,0,1,1,1,0,1,1,0,0,1,1,1,1,0,0,0,1,1,1,1,1,0,1,1,0,1,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,0,1,1,1,1,1,0,1,0,0,0,1,1,1,0,0,1,0,0,1,0,1,0,1,0,0,1,1,0,0,1,0,1,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,1,1,0,1,1,1,1,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,0,1,0,0,1,1,1,0,0,1,1,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,0,1,1,0,0,1,0,0,0,0,1,0,1,0,0,0,1,0,1,0,1,1,1,1,0,1,0,1,1,1,1,1,0,1,0,1,1,1,1,0,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,0,1,0,0,0,0,0,1,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,0,0,1,1,0,0,0,0,0,1,0,0,1,1,0,0,0,1,1,1,0,0,0,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,1,0,1,1,1,0,1,1,1,0,0,1,1,0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,0,0,0,0,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,0,0,1,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,0,0,1,0,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,1,0,0,1,0,0,0,1,0,1,0,0,1,0,0,1,0,0,0,0,0,1,1,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0,1,1,1,1,0,1,1,0,0,0,1,0,0,1,0,1,0,1,1,0,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,0,1,0,0,0,1,1,1,0,1,0,1,0,0,0,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,1,0,0,1,1,1,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,0,1,0,0,1,1,0,0,1,0,0,1,0,0,1,1,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,1,0,0,0,0,1,1,0,0,0,0,0,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,0,1,0,0,1,1,0,0,0,1,0,0,0,0,1,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,0,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,0,1,0,0,0,1,1,1,1,0,0,0,0,1,1,1,1,1,0,0,0,1,1,0,1,1,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,1,0,0,0,1,1,0,0,0,1,0,1,1,1,1,1,1,0,0,0,1,0,1,0,0,0,1,0,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,1,0,0,1,0,1,0,1,0,1,0,1,1,1,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,1,1,0,0,0,0,1,0,1,1,1,0,0,1,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,0,0,1,1,0,1,1,1,1,0,0,0,1,1,0,1,0,0,1,0,1,0,0,1,0,0,0,1,1,1,0,0,0,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,0,0,0,1,1,0,0,0,1,0,0,1,1,0,1,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,0,0,1,1,1,1,1,0,1,1,0,0,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,1,1,0,0,1,0,0,1,1,1,1,0,1,1,0,1,1,1,0,0,1,0,1,1,1,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,0,0,0,1,1,0,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,0,0,0,0,1,1,0,1,1,0,0,1,1,0,1,1,1,0,0,0,1,0,1,1,1,1,0,1,0,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,1,1,0,0,0,0,0,0,1,0,1,1,1,0,1,0,0,0,1,1,1,0,0,0,1,1,0,1,0,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,1,0,1,0,0,1,0,1,0,1,0,1,0,0,0,0,0,1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,1,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,1,1,1,0,1,0,0,0,1,1,0,0,1,1,1,1,0,1,1,1,1,0,0,1,1,1,0,1,1,1,1,1,1,1,0,0,0,1,0,0,0,0,0,0,1,0,0,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,1,1,0,0,1,0,1,0,1,1,1,0,1,1,0,0,0,0,1,0,0,1,0,1,1,0,0,1,1,0,0,1,0,0,1,0,1,1,0,0,0,1,1,0,0,1,0,1,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,0,1,1,0,0,0,1,1,1,1,1,1,1,0,1,0,1,1,0,1,1,1,1,1,1,0,1,1,1,0,0,1,0,1,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,1,0,0,1,0,1,0,1,0,1,1,0,0,0,0,1,0,1,0,1,1,1,0,1,0,0,0,0,0,1,1,0,0,1,0,1,0,0,1,0,0,0,0,0,0,1,0,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,1,0,1,0,1,1,1,1,0,1,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,1,0,0,1,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,0,0,1,0,0,0,0,1,0,1,1,0,0,0,0,0,0,1,1,0,1,0,0,1,1,1,0,0,0,1,1,0,1,0,0,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,0,1,1,0,1,0,0,1,1,1,1,1,1,1,0,1,1,0,0,1,0,0,1,1,0,1,0,1,0,0,0,0,1,0,0,1,1,1,0,0,0,1,0,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,0,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,1,0,1,0,1,0,0,1,1,1,0,0,0,0,0,0,1,1,0,0,0,1,1,0,0,0,0,0,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,0,0,1,0,0,0,0,1,0,0,1,1,1,1,1,0,0,1,0,0,0,1,1,0,0,1,0,0,1,0,1,1,0,1,0,0,1,1,1,1,0,0,0,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,1,0,1,0,1,0,0,1,0,1,0,0,0,0,0,1,1,0,1,1,1,0,0,0,1,1,1,0,0,0,0,0,1,0,0,1,1,1,0,0,1,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,1,1,0,0,0,1,0,0,0,0,0,0,0,1,1,0,1,1,1,1,0,0,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,1,1,0,0,0,0,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,0,1,1,1,0,1,0,1,0,0,1,0,0,1,0,0,0,1,0,1,1,1,0,0,0,0,0,1,0,1,0,1,1,0,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,0,1,1,1,0,0,0,0,1,1,0,0,0,0,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,0,0,0,1,1,0,0,1,1,1,0,0,0,0,1,0,1,0,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,1,0,1,0,1,1,1,1,1,1,0,0,1,0,0,1,0,0,0,0,1,1,0,1,0,1,0,1,1,0,1,1,0,1,0,0,1,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,1,1,1,0,1,0,0,1,1,1,1,1,0,0,1,1,1,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,0,1,0,1,0,1,0,1,0,0,0,0,1,1,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,0,0,1,1,0,0,0,0,0,1,1,0,1,0,1,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,1,0,1,1,1,0,1,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,0,0,1,1,1,0,0,0,0,1,1,1,0,0,1,0,1,1,0,1,0,1,0,1,0,0,0,1,1,0,0,0,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,0,1,1,1,0,1,0,0,1,1,1,1,0,0,0,1,0,0,0,1,0,0,1,1,1,0,0,0,0,1,0,1,1,1,0,1,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,1,1,1,0,0,1,1,0,1,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,0,0,1,0,1,1,1,1,1,0,0,1,1,1,0,0,0,0,1,1,0,1,1,0,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,0,0,1,1,0,0,1,1,1,0,1,0,1,0,1,1,0,1,0,0,0,1,1,0,1,1,0,0,1,1,0,0,1,1,0,0,1,0,1,1,0,0,0,0,0,0,0,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,0,1,0,1,1,0,1,1,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,1,0,0,0,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,1,0,1,0,0,1,0,1,1,0,0,1,1,0,1,0,0,0,1,0,1,1,1,1,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,1,1,0,1,0,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,1,0,1,0,1,0,0,1,1,0,0,0,0,1,1,0,0,1,0,0,0,0,1,0,0,0,1,0,0,0,1,1,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,0,1,0,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1,1,1,1,0,1,0,0,0,0,0,0,1,1,0,1,1,0,0,1,0,1,1,0,0,1,0,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,1,1,0,0,1,0,0,0,0,1,1,1,0,0,0,0,1,0,0,0,0,1,0,1,0,0,1,1,1,1,1,1,1,1,0,1,1,1,1,1,1,0,0,1,1,1,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,0,0,0,0,1,0,0,1,1,1,1,0,1,1,1,0,0,1,0,1,1,0,1,1,0,1,1,0,1,0,0,0,1,0,0,0,1,1,1,1,0,0,0,0,0,1,1,1,0,1,0,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,1,0,1,1,0,1,0,1,0,1,0,1,0,1,1,1,0,1,1,0,1,1,0,1,0,1,0,1,0,1,0,0,0,1,0,0,1,1,0,0,1,0,1,1,0,1,1,1,1,0,1,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,1,0,1,1,0,1,1,0,1,0,0,1,1,0,0,0,1,1,1,1,1,1,0,0,0,1,0,1,0,1,1,0,0,0,1,1,1,0,1,0,0,0,1,0,1,1,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,0,1,0,0,0,1,1,1,0,1,1,0,1,0,0,0,0,0,0,1,0,0,1,1,0,1,1,0,0,1,0,0,0,0,1,1,1,1,0,0,1,1,0,1,0,0,0,1,1,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,1,1,1,1,0,0,1,1,0,0,0,1,0,1,1,0,0,1,0,0,0,0,0,0,0,1,1,0,0,0,1,0,0,0,0,1,0,0,1,1,0,1,0,0,1,0,0,0,0,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[0,0,1,0,0,0,1,0,0,1,1,0,0,0,0,1,1,1,0,1,0,0,0,1,0,1,0,1,1,0,0,1,0,1,1,0,1,1,0,1,0,1,1,0,0,0,1,1,1,1,0,0,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,0,1,0,0,1,0,0,1,0,1,0,1,0,1,1,1,0,0,1,0,0,1,1,0,1,1,0,0,0,1,1,1,0,0,1,0,0,1,0,0,1,1,1,0,0,1,1,0,1,1,1,1,1,1,1,1,1,1,1,1]</t>
+  </si>
+  <si>
+    <t>[1,1,0,1,1,1,1,0,1,0,1,1,0,1,1,1,0,0,0,0,0,1,1,0,1,0,0,0,1,1,0,1,0,0,0,1,1,0,0,1,0,0,1,0,0,0,1,0,0,0,1,0,1,0,1,1,1,1,1,1,1]</t>
   </si>
 </sst>
 </file>
@@ -658,10 +550,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -961,10 +849,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-  <dimension ref="A1:C90"/>
+  <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C90"/>
+    <sheetView tabSelected="1" topLeftCell="A63" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73:C90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -991,7 +879,7 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -1002,7 +890,7 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -1013,7 +901,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>100</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
@@ -1024,7 +912,7 @@
         <v>5</v>
       </c>
       <c r="C5" t="s">
-        <v>101</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -1035,7 +923,7 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -1046,7 +934,7 @@
         <v>5</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -1057,7 +945,7 @@
         <v>5</v>
       </c>
       <c r="C8" t="s">
-        <v>104</v>
+        <v>86</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -1068,7 +956,7 @@
         <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>105</v>
+        <v>87</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -1079,7 +967,7 @@
         <v>5</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
@@ -1090,7 +978,7 @@
         <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -1101,7 +989,7 @@
         <v>7</v>
       </c>
       <c r="C12" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
@@ -1112,7 +1000,7 @@
         <v>7</v>
       </c>
       <c r="C13" t="s">
-        <v>109</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -1123,7 +1011,7 @@
         <v>7</v>
       </c>
       <c r="C14" t="s">
-        <v>110</v>
+        <v>92</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
@@ -1134,7 +1022,7 @@
         <v>7</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
@@ -1145,7 +1033,7 @@
         <v>7</v>
       </c>
       <c r="C16" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
@@ -1156,7 +1044,7 @@
         <v>7</v>
       </c>
       <c r="C17" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
@@ -1167,7 +1055,7 @@
         <v>7</v>
       </c>
       <c r="C18" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
@@ -1178,7 +1066,7 @@
         <v>7</v>
       </c>
       <c r="C19" t="s">
-        <v>115</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -1189,7 +1077,7 @@
         <v>7</v>
       </c>
       <c r="C20" t="s">
-        <v>116</v>
+        <v>98</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
@@ -1200,7 +1088,7 @@
         <v>6</v>
       </c>
       <c r="C21" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
@@ -1211,7 +1099,7 @@
         <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>118</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
@@ -1222,7 +1110,7 @@
         <v>6</v>
       </c>
       <c r="C23" t="s">
-        <v>119</v>
+        <v>101</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -1233,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>120</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
@@ -1244,7 +1132,7 @@
         <v>6</v>
       </c>
       <c r="C25" t="s">
-        <v>121</v>
+        <v>103</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
@@ -1255,7 +1143,7 @@
         <v>6</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
@@ -1266,7 +1154,7 @@
         <v>6</v>
       </c>
       <c r="C27" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.3">
@@ -1277,7 +1165,7 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>124</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.3">
@@ -1288,7 +1176,7 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>125</v>
+        <v>107</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.3">
@@ -1299,7 +1187,7 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>126</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.3">
@@ -1310,7 +1198,7 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>127</v>
+        <v>109</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.3">
@@ -1321,7 +1209,7 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>128</v>
+        <v>110</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
@@ -1332,7 +1220,7 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
@@ -1343,7 +1231,7 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
@@ -1354,7 +1242,7 @@
         <v>4</v>
       </c>
       <c r="C35" t="s">
-        <v>131</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
@@ -1365,7 +1253,7 @@
         <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>132</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
@@ -1376,7 +1264,7 @@
         <v>4</v>
       </c>
       <c r="C37" t="s">
-        <v>133</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
@@ -1387,7 +1275,7 @@
         <v>4</v>
       </c>
       <c r="C38" t="s">
-        <v>134</v>
+        <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
@@ -1398,7 +1286,7 @@
         <v>4</v>
       </c>
       <c r="C39" t="s">
-        <v>135</v>
+        <v>117</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
@@ -1409,7 +1297,7 @@
         <v>4</v>
       </c>
       <c r="C40" t="s">
-        <v>136</v>
+        <v>118</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.3">
@@ -1420,7 +1308,7 @@
         <v>4</v>
       </c>
       <c r="C41" t="s">
-        <v>137</v>
+        <v>119</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
@@ -1431,7 +1319,7 @@
         <v>4</v>
       </c>
       <c r="C42" t="s">
-        <v>138</v>
+        <v>120</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.3">
@@ -1442,7 +1330,7 @@
         <v>8</v>
       </c>
       <c r="C43" t="s">
-        <v>139</v>
+        <v>121</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
@@ -1453,7 +1341,7 @@
         <v>8</v>
       </c>
       <c r="C44" t="s">
-        <v>140</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
@@ -1464,7 +1352,7 @@
         <v>8</v>
       </c>
       <c r="C45" t="s">
-        <v>141</v>
+        <v>123</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
@@ -1475,7 +1363,7 @@
         <v>8</v>
       </c>
       <c r="C46" t="s">
-        <v>142</v>
+        <v>124</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.3">
@@ -1486,7 +1374,7 @@
         <v>8</v>
       </c>
       <c r="C47" t="s">
-        <v>143</v>
+        <v>125</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.3">
@@ -1497,7 +1385,7 @@
         <v>8</v>
       </c>
       <c r="C48" t="s">
-        <v>144</v>
+        <v>126</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
@@ -1508,7 +1396,7 @@
         <v>8</v>
       </c>
       <c r="C49" t="s">
-        <v>145</v>
+        <v>127</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
@@ -1519,7 +1407,7 @@
         <v>8</v>
       </c>
       <c r="C50" t="s">
-        <v>146</v>
+        <v>128</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.3">
@@ -1530,7 +1418,7 @@
         <v>8</v>
       </c>
       <c r="C51" t="s">
-        <v>147</v>
+        <v>129</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.3">
@@ -1541,7 +1429,7 @@
         <v>8</v>
       </c>
       <c r="C52" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
@@ -1552,7 +1440,7 @@
         <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
@@ -1563,7 +1451,7 @@
         <v>8</v>
       </c>
       <c r="C54" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
@@ -1574,7 +1462,7 @@
         <v>8</v>
       </c>
       <c r="C55" t="s">
-        <v>151</v>
+        <v>133</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
@@ -1585,7 +1473,7 @@
         <v>8</v>
       </c>
       <c r="C56" t="s">
-        <v>152</v>
+        <v>134</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
@@ -1596,7 +1484,7 @@
         <v>8</v>
       </c>
       <c r="C57" t="s">
-        <v>153</v>
+        <v>135</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
@@ -1607,7 +1495,7 @@
         <v>8</v>
       </c>
       <c r="C58" t="s">
-        <v>154</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
@@ -1618,7 +1506,7 @@
         <v>8</v>
       </c>
       <c r="C59" t="s">
-        <v>155</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
@@ -1629,7 +1517,7 @@
         <v>8</v>
       </c>
       <c r="C60" t="s">
-        <v>156</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
@@ -1640,7 +1528,7 @@
         <v>8</v>
       </c>
       <c r="C61" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
@@ -1651,7 +1539,7 @@
         <v>8</v>
       </c>
       <c r="C62" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
@@ -1662,7 +1550,7 @@
         <v>8</v>
       </c>
       <c r="C63" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
@@ -1673,7 +1561,7 @@
         <v>8</v>
       </c>
       <c r="C64" t="s">
-        <v>160</v>
+        <v>142</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
@@ -1684,7 +1572,7 @@
         <v>8</v>
       </c>
       <c r="C65" t="s">
-        <v>161</v>
+        <v>143</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
@@ -1695,7 +1583,7 @@
         <v>8</v>
       </c>
       <c r="C66" t="s">
-        <v>162</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
@@ -1706,7 +1594,7 @@
         <v>8</v>
       </c>
       <c r="C67" t="s">
-        <v>163</v>
+        <v>145</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
@@ -1717,7 +1605,7 @@
         <v>8</v>
       </c>
       <c r="C68" t="s">
-        <v>164</v>
+        <v>146</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
@@ -1728,7 +1616,7 @@
         <v>8</v>
       </c>
       <c r="C69" t="s">
-        <v>165</v>
+        <v>147</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
@@ -1739,7 +1627,7 @@
         <v>8</v>
       </c>
       <c r="C70" t="s">
-        <v>166</v>
+        <v>148</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
@@ -1750,7 +1638,7 @@
         <v>8</v>
       </c>
       <c r="C71" t="s">
-        <v>167</v>
+        <v>149</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
@@ -1761,210 +1649,12 @@
         <v>8</v>
       </c>
       <c r="C72" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" t="s">
-        <v>80</v>
-      </c>
-      <c r="B73" t="s">
-        <v>8</v>
-      </c>
-      <c r="C73" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" t="s">
-        <v>81</v>
-      </c>
-      <c r="B74" t="s">
-        <v>8</v>
-      </c>
-      <c r="C74" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" t="s">
-        <v>82</v>
-      </c>
-      <c r="B75" t="s">
-        <v>8</v>
-      </c>
-      <c r="C75" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" t="s">
-        <v>83</v>
-      </c>
-      <c r="B76" t="s">
-        <v>8</v>
-      </c>
-      <c r="C76" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" t="s">
-        <v>84</v>
-      </c>
-      <c r="B77" t="s">
-        <v>8</v>
-      </c>
-      <c r="C77" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" t="s">
-        <v>85</v>
-      </c>
-      <c r="B78" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" t="s">
-        <v>174</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" t="s">
-        <v>86</v>
-      </c>
-      <c r="B79" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" t="s">
-        <v>87</v>
-      </c>
-      <c r="B80" t="s">
-        <v>8</v>
-      </c>
-      <c r="C80" t="s">
-        <v>176</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" t="s">
-        <v>88</v>
-      </c>
-      <c r="B81" t="s">
-        <v>8</v>
-      </c>
-      <c r="C81" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" t="s">
-        <v>89</v>
-      </c>
-      <c r="B82" t="s">
-        <v>8</v>
-      </c>
-      <c r="C82" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" t="s">
-        <v>90</v>
-      </c>
-      <c r="B83" t="s">
-        <v>8</v>
-      </c>
-      <c r="C83" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" t="s">
-        <v>91</v>
-      </c>
-      <c r="B84" t="s">
-        <v>8</v>
-      </c>
-      <c r="C84" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" t="s">
-        <v>92</v>
-      </c>
-      <c r="B85" t="s">
-        <v>8</v>
-      </c>
-      <c r="C85" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" t="s">
-        <v>93</v>
-      </c>
-      <c r="B86" t="s">
-        <v>8</v>
-      </c>
-      <c r="C86" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" t="s">
-        <v>94</v>
-      </c>
-      <c r="B87" t="s">
-        <v>8</v>
-      </c>
-      <c r="C87" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" t="s">
-        <v>95</v>
-      </c>
-      <c r="B88" t="s">
-        <v>8</v>
-      </c>
-      <c r="C88" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" t="s">
-        <v>96</v>
-      </c>
-      <c r="B89" t="s">
-        <v>8</v>
-      </c>
-      <c r="C89" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" t="s">
-        <v>97</v>
-      </c>
-      <c r="B90" t="s">
-        <v>8</v>
-      </c>
-      <c r="C90" t="s">
-        <v>186</v>
+        <v>150</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C74" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C74">
+  <autoFilter ref="A1:C72" xr:uid="{02B8EB59-0594-4E0B-8CEE-7326F1E18A00}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C72">
       <sortCondition ref="A1"/>
     </sortState>
   </autoFilter>

</xml_diff>